<commit_message>
cambio de Provedor y Cliente Karina
</commit_message>
<xml_diff>
--- a/SistemaInventario/Reportes/Xls_Productos_Aplicacion.xlsx
+++ b/SistemaInventario/Reportes/Xls_Productos_Aplicacion.xlsx
@@ -33,30 +33,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>REPORTE PRODUCTO APLICACION</t>
   </si>
   <si>
-    <t>NroRuc</t>
-  </si>
-  <si>
-    <t>RazonSocial</t>
+    <t>Documento</t>
+  </si>
+  <si>
+    <t>Cliente</t>
   </si>
   <si>
     <t>NombreComercial</t>
   </si>
   <si>
-    <t>FlagRetencion</t>
-  </si>
-  <si>
-    <t>FlagBloqueoCredito</t>
+    <t>Retencion</t>
+  </si>
+  <si>
+    <t>BloqueoCredito</t>
   </si>
   <si>
     <t>Distrito</t>
   </si>
   <si>
     <t>Direccion</t>
+  </si>
+  <si>
+    <t>10176022197</t>
+  </si>
+  <si>
+    <t>RIVERA CASTILLO ALEJANDRO MATEO</t>
+  </si>
+  <si>
+    <t>SAN MIGUEL</t>
+  </si>
+  <si>
+    <t>CAL. LOS NARANJALES MZA. M LOTE. 22 A.H. PANDO IX ET.</t>
   </si>
 </sst>
 </file>
@@ -420,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
@@ -462,6 +474,26 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:G1"/>

</xml_diff>

<commit_message>
Se acepta version del servidor en conflictos
</commit_message>
<xml_diff>
--- a/SistemaInventario/Reportes/Xls_Productos_Aplicacion.xlsx
+++ b/SistemaInventario/Reportes/Xls_Productos_Aplicacion.xlsx
@@ -33,42 +33,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>REPORTE PRODUCTO APLICACION</t>
   </si>
   <si>
-    <t>Documento</t>
-  </si>
-  <si>
-    <t>Cliente</t>
+    <t>NroRuc</t>
+  </si>
+  <si>
+    <t>RazonSocial</t>
   </si>
   <si>
     <t>NombreComercial</t>
   </si>
   <si>
-    <t>Retencion</t>
-  </si>
-  <si>
-    <t>BloqueoCredito</t>
+    <t>FlagRetencion</t>
+  </si>
+  <si>
+    <t>FlagBloqueoCredito</t>
   </si>
   <si>
     <t>Distrito</t>
   </si>
   <si>
     <t>Direccion</t>
-  </si>
-  <si>
-    <t>10176022197</t>
-  </si>
-  <si>
-    <t>RIVERA CASTILLO ALEJANDRO MATEO</t>
-  </si>
-  <si>
-    <t>SAN MIGUEL</t>
-  </si>
-  <si>
-    <t>CAL. LOS NARANJALES MZA. M LOTE. 22 A.H. PANDO IX ET.</t>
   </si>
 </sst>
 </file>
@@ -432,7 +420,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
@@ -474,26 +462,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:G1"/>

</xml_diff>

<commit_message>
franco excel y producto
</commit_message>
<xml_diff>
--- a/SistemaInventario/Reportes/Xls_Productos_Aplicacion.xlsx
+++ b/SistemaInventario/Reportes/Xls_Productos_Aplicacion.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FUENTESGIT\SGAE_2010\SistemaInventario\Reportes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SGAE_2010\SGAE_2010\SistemaInventario\Reportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Aplicacion" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,38 +33,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>REPORTE PRODUCTO APLICACION</t>
+    <t>REPORTE PRODUCTO</t>
   </si>
   <si>
-    <t>NroRuc</t>
+    <t>Fecha:</t>
   </si>
   <si>
-    <t>RazonSocial</t>
-  </si>
-  <si>
-    <t>NombreComercial</t>
-  </si>
-  <si>
-    <t>FlagRetencion</t>
-  </si>
-  <si>
-    <t>FlagBloqueoCredito</t>
-  </si>
-  <si>
-    <t>Distrito</t>
-  </si>
-  <si>
-    <t>Direccion</t>
+    <t>Cantidad de registros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,7 +58,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -99,13 +91,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,54 +414,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="23.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="I1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
-    <mergeCell ref="A1:G1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>